<commit_message>
Fix X_sqrt bug to X
</commit_message>
<xml_diff>
--- a/outputs/1 fusion results.xlsx
+++ b/outputs/1 fusion results.xlsx
@@ -782,7 +782,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="E1:M13"/>
+  <dimension ref="E1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1276,6 +1276,117 @@
         </is>
       </c>
       <c r="M13" t="inlineStr">
+        <is>
+          <t>[1, 0, 0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>00000</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>00001</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>0.3150710546445558</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.3150710546445558</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.3138200235949994</v>
+      </c>
+      <c r="J14" t="n">
+        <v>1.003986460249493</v>
+      </c>
+      <c r="K14" t="n">
+        <v>1.003986460249493</v>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>[1, 0, 0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>00000</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>00001</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>0.3150710546445558</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.3150710546445558</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.3138200235949994</v>
+      </c>
+      <c r="J15" t="n">
+        <v>1.003986460249493</v>
+      </c>
+      <c r="K15" t="n">
+        <v>1.003986460249493</v>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>[1, 0, 0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>00000</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>00001</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>0.3150710546445558</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.3150710546445558</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.3138200235949994</v>
+      </c>
+      <c r="J16" t="n">
+        <v>1.003986460249493</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1.003986460249493</v>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
         <is>
           <t>[1, 0, 0]</t>
         </is>
@@ -1292,7 +1403,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="E1:M13"/>
+  <dimension ref="E1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1786,6 +1897,117 @@
         </is>
       </c>
       <c r="M13" t="inlineStr">
+        <is>
+          <t>[0, 1, 0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>01000</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>00000</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>0.244540930063405</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.3714195878083486</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.244540930063405</v>
+      </c>
+      <c r="J14" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" t="n">
+        <v>1.518844259372229</v>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>[0, 1, 0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>01000</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>00000</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>0.244540930063405</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.3714195878083486</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.244540930063405</v>
+      </c>
+      <c r="J15" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" t="n">
+        <v>1.518844259372229</v>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>[0, 1, 0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>01000</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>00000</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>0.244540930063405</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.3714195878083486</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.244540930063405</v>
+      </c>
+      <c r="J16" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1.518844259372229</v>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
         <is>
           <t>[0, 1, 0]</t>
         </is>
@@ -1802,7 +2024,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="E1:M13"/>
+  <dimension ref="E1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2301,6 +2523,117 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>00001</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>00000</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>0.1996668332936564</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.3446822454299492</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.1996668332936564</v>
+      </c>
+      <c r="J14" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" t="n">
+        <v>1.726286933809452</v>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>[0, 0, 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>00001</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>00000</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>0.1996668332936564</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.3446822454299492</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.1996668332936564</v>
+      </c>
+      <c r="J15" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" t="n">
+        <v>1.726286933809452</v>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>[0, 0, 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>00001</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>00000</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>0.1996668332936564</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.3446822454299492</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.1996668332936564</v>
+      </c>
+      <c r="J16" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" t="n">
+        <v>1.726286933809452</v>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>0.2</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>[0, 0, 1]</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>